<commit_message>
till now - GOOD !!!!
</commit_message>
<xml_diff>
--- a/Plan/TO-DOs.xlsx
+++ b/Plan/TO-DOs.xlsx
@@ -12,14 +12,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$D$15</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$D$16</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>Accommodate for option type and strike price along with symbol in option price capture component</t>
   </si>
@@ -423,11 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="1"/>
   <dimension ref="A2:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.85546875" defaultRowHeight="15"/>
@@ -457,7 +456,10 @@
         <v>0</v>
       </c>
       <c r="C3" s="1">
-        <v>1</v>
+        <v>10</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="45">
@@ -468,7 +470,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>21</v>
@@ -482,13 +484,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="150" hidden="1">
+    <row r="6" spans="1:4" ht="150">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -502,7 +504,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:4" hidden="1">
+    <row r="7" spans="1:4">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -513,7 +515,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" hidden="1">
+    <row r="8" spans="1:4">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -524,7 +526,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:4" hidden="1">
+    <row r="9" spans="1:4">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -535,7 +537,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" hidden="1">
+    <row r="10" spans="1:4">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -554,13 +556,13 @@
         <v>7</v>
       </c>
       <c r="C11" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:4" hidden="1">
+    <row r="12" spans="1:4">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -571,7 +573,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:4" hidden="1">
+    <row r="13" spans="1:4">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -596,7 +598,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="30" hidden="1">
+    <row r="15" spans="1:4" ht="30">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -619,13 +621,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:D15">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="1"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A2:D16"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
corrected option extraction code and made good changes to queries files
</commit_message>
<xml_diff>
--- a/Plan/TO-DOs.xlsx
+++ b/Plan/TO-DOs.xlsx
@@ -461,8 +461,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A2:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.85546875" defaultRowHeight="15"/>
@@ -700,7 +700,7 @@
     </row>
     <row r="19" spans="1:6" ht="30">
       <c r="A19" s="1">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
implemented logic to calculate order factor from selected instrument
</commit_message>
<xml_diff>
--- a/Plan/TO-DOs.xlsx
+++ b/Plan/TO-DOs.xlsx
@@ -12,14 +12,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$D$21</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$D$23</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="41">
   <si>
     <t>Accommodate for option type and strike price along with symbol in option price capture component</t>
   </si>
@@ -136,6 +136,20 @@
   </si>
   <si>
     <t>Done for now</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Change buy and sell order factor - calculate factor from dummy option price calculation
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MONITOR - Check if option prices data saving pauses - aim for single websocket and worker threads to extract data
+</t>
+  </si>
+  <si>
+    <t>Capture High Price in option price data</t>
+  </si>
+  <si>
+    <t>Limit Buy order price to 75 % of high price</t>
   </si>
 </sst>
 </file>
@@ -470,10 +484,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:F21"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A2:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.85546875" defaultRowHeight="15"/>
@@ -497,7 +512,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="60">
+    <row r="3" spans="1:5" ht="60" hidden="1">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -511,7 +526,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="45">
+    <row r="4" spans="1:5" ht="45" hidden="1">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -519,13 +534,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="45">
+    <row r="5" spans="1:5" ht="45" hidden="1">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -539,7 +554,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="150">
+    <row r="6" spans="1:5" ht="150" hidden="1">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -547,7 +562,7 @@
         <v>9</v>
       </c>
       <c r="C6" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>16</v>
@@ -561,13 +576,13 @@
         <v>3</v>
       </c>
       <c r="C7" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" hidden="1">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -578,7 +593,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" hidden="1">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -592,7 +607,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" hidden="1">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -606,7 +621,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="30">
+    <row r="11" spans="1:5" ht="30" hidden="1">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -628,10 +643,10 @@
         <v>8</v>
       </c>
       <c r="C12" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="30" hidden="1">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -639,13 +654,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="45">
+    <row r="14" spans="1:5" ht="45" hidden="1">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -653,7 +668,7 @@
         <v>15</v>
       </c>
       <c r="C14" s="1">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>33</v>
@@ -662,7 +677,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="30">
+    <row r="15" spans="1:5" ht="30" hidden="1">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -679,7 +694,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="30">
+    <row r="16" spans="1:5" ht="30" hidden="1">
       <c r="A16" s="1">
         <v>13</v>
       </c>
@@ -693,7 +708,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="30">
+    <row r="17" spans="1:6" ht="30" hidden="1">
       <c r="A17" s="1">
         <v>14</v>
       </c>
@@ -701,7 +716,7 @@
         <v>22</v>
       </c>
       <c r="C17" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>28</v>
@@ -710,7 +725,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="60">
+    <row r="18" spans="1:6" ht="60" hidden="1">
       <c r="A18" s="1">
         <v>15</v>
       </c>
@@ -730,7 +745,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="30">
+    <row r="19" spans="1:6" ht="30" hidden="1">
       <c r="A19" s="1">
         <v>16</v>
       </c>
@@ -755,10 +770,10 @@
         <v>29</v>
       </c>
       <c r="C20" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" hidden="1">
       <c r="A21" s="1">
         <v>18</v>
       </c>
@@ -772,9 +787,46 @@
         <v>30</v>
       </c>
     </row>
+    <row r="22" spans="1:6" ht="60">
+      <c r="B22" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="75">
+      <c r="B23" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="30">
+      <c r="B24" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="30">
+      <c r="B25" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25" s="1">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A2:D21">
-    <filterColumn colId="2"/>
+  <autoFilter ref="A2:D23">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="1"/>
+        <filter val="2"/>
+      </filters>
+    </filterColumn>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>